<commit_message>
Updates to several slides.
</commit_message>
<xml_diff>
--- a/notes/Campaign Manager Backlog 10022014.xlsx
+++ b/notes/Campaign Manager Backlog 10022014.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="480" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="1880" yWindow="480" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Campaign Manager" sheetId="1" r:id="rId1"/>
@@ -405,19 +405,19 @@
     <t>Validate user configuration upon login</t>
   </si>
   <si>
-    <t>Road Map (12-24 Weeks) Not for 2/1</t>
-  </si>
-  <si>
-    <t>(7-11 weeks) To be evaluated for 2/1</t>
-  </si>
-  <si>
-    <t>Wish List</t>
-  </si>
-  <si>
     <t>Strategy (24+ Weeks)</t>
   </si>
   <si>
     <t>Incoropriate require.js</t>
+  </si>
+  <si>
+    <t>(7-11 weeks)</t>
+  </si>
+  <si>
+    <t>Road Map (12-24 Weeks)</t>
+  </si>
+  <si>
+    <t>Wish List/Requests</t>
   </si>
 </sst>
 </file>
@@ -1786,8 +1786,8 @@
   <dimension ref="A1:F149"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A70" sqref="A70"/>
+      <pane ySplit="1" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A137" sqref="A137:E137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2139,7 +2139,7 @@
         <v>5</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E23" s="11">
         <v>21</v>
@@ -2485,7 +2485,7 @@
     </row>
     <row r="48" spans="1:6" ht="19" thickBot="1">
       <c r="A48" s="117" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B48" s="118"/>
       <c r="C48" s="118"/>
@@ -3229,7 +3229,7 @@
     </row>
     <row r="101" spans="1:6" ht="19" thickBot="1">
       <c r="A101" s="117" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B101" s="118"/>
       <c r="C101" s="118"/>
@@ -3327,7 +3327,7 @@
     </row>
     <row r="110" spans="1:6" ht="19" thickBot="1">
       <c r="A110" s="111" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B110" s="112"/>
       <c r="C110" s="112"/>
@@ -3599,7 +3599,7 @@
     </row>
     <row r="137" spans="1:6" ht="19" thickBot="1">
       <c r="A137" s="111" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B137" s="112"/>
       <c r="C137" s="112"/>

</xml_diff>